<commit_message>
Presentado 3T y cuentas OB revisadas. Pdte. rev. trasn. auto
</commit_message>
<xml_diff>
--- a/AEAT/LibroMaestro.xlsx
+++ b/AEAT/LibroMaestro.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\gestoria\AEAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D62613-3004-4CA2-A3DB-BB88AA4ADC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FFDFBB-67BE-4BE4-82AE-B48FC1C7450A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19308" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{3DFA84EE-35D1-40DB-9C01-33D82470448C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="16220" windowHeight="8620" xr2:uid="{3DFA84EE-35D1-40DB-9C01-33D82470448C}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckList" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Mod 130" sheetId="2" r:id="rId2"/>
+    <sheet name="Ventas Libro" sheetId="4" r:id="rId3"/>
+    <sheet name="Gastos" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>📊 Checklist Trimestral Autónomos – 3T 2025</t>
   </si>
@@ -85,13 +90,163 @@
   </si>
   <si>
     <t>❌ Solo si contrato sujeto a retención</t>
+  </si>
+  <si>
+    <t>1T</t>
+  </si>
+  <si>
+    <t>Rendimiento neto</t>
+  </si>
+  <si>
+    <t>Casilla</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Rtdo Autoliquidacion</t>
+  </si>
+  <si>
+    <t>2T</t>
+  </si>
+  <si>
+    <t>Desglose ventas:</t>
+  </si>
+  <si>
+    <t>Regalías Amazon. Periodo febrero</t>
+  </si>
+  <si>
+    <t>Amazon cobrado febrero</t>
+  </si>
+  <si>
+    <t>Detalle de Gastos</t>
+  </si>
+  <si>
+    <t>Borax</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Iva</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>CD Mon</t>
+  </si>
+  <si>
+    <t>Total 1T</t>
+  </si>
+  <si>
+    <t>Facturas iva 21%</t>
+  </si>
+  <si>
+    <t>Mod 130 Ingresos</t>
+  </si>
+  <si>
+    <t>Mod 130 Gastos</t>
+  </si>
+  <si>
+    <t>Disco SSD</t>
+  </si>
+  <si>
+    <t>Hosting slicingpie.es hasta 30/4/26</t>
+  </si>
+  <si>
+    <t>diferencia</t>
+  </si>
+  <si>
+    <t>3T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFERENCIA DE AMAZON.COM SERVICES LLC, CONCEPTO TLR002892917042 PO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFERENCIA DE AMAZON MEDIA EU S.A R.L., CONCEPTO FCS002839125762 PAYMENT-NUM 3 33988842 </t>
+  </si>
+  <si>
+    <t>Casilla 01</t>
+  </si>
+  <si>
+    <t>Total Amazon 2T</t>
+  </si>
+  <si>
+    <t>Cuotas Autonomos</t>
+  </si>
+  <si>
+    <t>Suma Gastos</t>
+  </si>
+  <si>
+    <t>Casilla 02</t>
+  </si>
+  <si>
+    <t>Cuota</t>
+  </si>
+  <si>
+    <t>Cuota sin bonificaion (sin recargo)</t>
+  </si>
+  <si>
+    <t>Total Cuotas 2T</t>
+  </si>
+  <si>
+    <t>Cuotas IA GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuotas aut 3T </t>
+  </si>
+  <si>
+    <t>Cuota julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA DE Stripe Technology Europe Ltd, CONCEPTO STRIPE Q0K7G9</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA DE AMAZON.COM SERVICES LLC, CONCEPTO TLR003029611492 PO</t>
+  </si>
+  <si>
+    <t>Suma Ventas</t>
+  </si>
+  <si>
+    <t>Total Amazon y Stripe  3T</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Importante: en el 4T averiguar tratamiento de ventas en el IVA y regularizar el resto del año</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-C0A]dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +278,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,11 +313,58 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -145,7 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -160,6 +388,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -178,6 +442,46 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Posicion"/>
+      <sheetName val="5382 CC Ed"/>
+      <sheetName val="8017 Gtos Piso"/>
+      <sheetName val="2663 Alquiler"/>
+      <sheetName val="7572 Personal"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="31">
+          <cell r="K31" t="str">
+            <v>IA Github</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="H45">
+            <v>6.76</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="H55">
+            <v>-8.56</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,26 +801,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34686593-8238-4488-AFF3-0D03C3E38067}">
-  <dimension ref="B3:G10"/>
+  <dimension ref="B3:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="6" max="6" width="36.296875" customWidth="1"/>
-    <col min="7" max="7" width="20.59765625" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="17.399999999999999">
+    <row r="3" spans="2:7" ht="17.5">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="27.6">
+    <row r="5" spans="2:7" ht="28">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -536,7 +840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="28.2" customHeight="1">
+    <row r="6" spans="2:7" ht="28.25" customHeight="1">
       <c r="B6" s="4">
         <v>303</v>
       </c>
@@ -547,7 +851,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -567,14 +871,14 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="2:7" ht="4.8" customHeight="1">
+    <row r="8" spans="2:7" ht="4.75" customHeight="1">
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:7" ht="41.4">
+    <row r="9" spans="2:7" ht="28">
       <c r="B9" s="4">
         <v>111</v>
       </c>
@@ -587,7 +891,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:7" ht="41.4">
+    <row r="10" spans="2:7" ht="28">
       <c r="B10" s="4">
         <v>115</v>
       </c>
@@ -599,6 +903,11 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -610,14 +919,518 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F379C0C-D679-4DB5-89CA-EC448EC63179}">
-  <dimension ref="A1"/>
+  <dimension ref="B5:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:7">
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>11.49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>10.54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="10">
+        <f>+SUM(D7:D9)</f>
+        <v>34.090000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <f>+D13-D10</f>
+        <v>6.9399999999999977</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>41.03</v>
+      </c>
+      <c r="E13">
+        <f>+'Ventas Libro'!C7</f>
+        <v>17.5</v>
+      </c>
+      <c r="F13">
+        <f>+'Ventas Libro'!C12</f>
+        <v>16.18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="6"/>
+      <c r="F14">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16">
+        <f>+Gastos!C7</f>
+        <v>146.21</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="E17">
+        <f>87.61*2</f>
+        <v>175.22</v>
+      </c>
+      <c r="F17">
+        <f>+Gastos!E19</f>
+        <v>262.83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19">
+        <f>+SUM(D16:D17)</f>
+        <v>146.21</v>
+      </c>
+      <c r="E19">
+        <f>+SUM(E16:E17)</f>
+        <v>175.22</v>
+      </c>
+      <c r="F19">
+        <f>+SUM(F16:F17)</f>
+        <v>262.83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>146.21</v>
+      </c>
+      <c r="E21">
+        <v>464.33</v>
+      </c>
+      <c r="F21">
+        <f>+F19</f>
+        <v>262.83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <f>+D13-D21</f>
+        <v>-105.18</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:F23" si="0">+E13-E21</f>
+        <v>-446.83</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>-246.64999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF305462-E993-4620-8A0E-C96086C1FA84}">
+  <dimension ref="A4:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="38.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25">
+      <c r="A5" s="12">
+        <v>45806</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="14">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48.5" customHeight="1">
+      <c r="A6" s="12">
+        <v>45776</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="14">
+        <v>10.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <f>+C5+C6</f>
+        <v>17.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25">
+      <c r="A10" s="16">
+        <v>45936</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="17">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25">
+      <c r="A11" s="8">
+        <v>45867</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <f>+'[1]5382 CC Ed'!$H$45</f>
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="19">
+        <f>+SUM(C10:C11)</f>
+        <v>16.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827477B7-78E6-4C9E-8644-45F411C08776}">
+  <dimension ref="A3:G26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="8">
+        <v>45665</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>62.81</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="E4">
+        <f>+D4*C4</f>
+        <v>13.190099999999999</v>
+      </c>
+      <c r="F4">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="8">
+        <v>45737</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>83.4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="E5">
+        <f>+D5*C5</f>
+        <v>17.513999999999999</v>
+      </c>
+      <c r="F5">
+        <v>100.91</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <f>+SUM(C4:C6)</f>
+        <v>146.21</v>
+      </c>
+      <c r="E7">
+        <f>+SUM(E4:E6)</f>
+        <v>30.704099999999997</v>
+      </c>
+      <c r="F7">
+        <f>+SUM(F4:F6)</f>
+        <v>176.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="12">
+        <v>45838</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="14">
+        <v>-87.61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="8">
+        <v>45807</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="14">
+        <v>-87.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="15">
+        <v>45748</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <v>-289.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <f>+SUM(E13:E15)</f>
+        <v>-464.33000000000004</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19">
+        <f>87.61*3</f>
+        <v>262.83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="str">
+        <f>+'[1]5382 CC Ed'!$K$31</f>
+        <v>IA Github</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="8">
+        <v>45839</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23">
+        <f>+'[1]5382 CC Ed'!$H$55</f>
+        <v>-8.56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="16">
+        <v>45869</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="17">
+        <v>-8.6199999999999992</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="16">
+        <v>45901</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="18">
+        <v>-8.61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="D26" s="19">
+        <f>+SUM(D23:D25)</f>
+        <v>-25.79</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>